<commit_message>
Recibo Nacional - Recibo combinado
</commit_message>
<xml_diff>
--- a/src/Data/DataTest.xlsx
+++ b/src/Data/DataTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Pedido</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>CC000001318023</t>
+  </si>
+  <si>
+    <t>Pedido Nacional Comb - METROMALL</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>EMPAQUE</t>
+  </si>
+  <si>
+    <t>M005</t>
+  </si>
+  <si>
+    <t>Centro PPK</t>
   </si>
 </sst>
 </file>
@@ -119,12 +134,18 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,10 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +459,7 @@
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -488,10 +511,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4500144645</v>
+        <v>4500144688</v>
       </c>
       <c r="B3" s="1">
-        <v>7450043069770</v>
+        <v>7450043069886</v>
       </c>
       <c r="C3" s="1"/>
       <c r="G3" s="1">
@@ -574,7 +597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4500144675</v>
       </c>
@@ -591,7 +614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -604,8 +627,11 @@
       <c r="F20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4500144685</v>
       </c>
@@ -624,17 +650,54 @@
       <c r="F21">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>4500144611</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4500144684</v>
+        <v>4500144691</v>
       </c>
       <c r="B22" s="1">
-        <v>2040000639167</v>
-      </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2040000642174</v>
+      </c>
+      <c r="C22" s="1">
+        <v>380</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="1">
+        <v>7611501611195</v>
+      </c>
+      <c r="I23">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <v>12</v>
+      </c>
+      <c r="K23" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4500144686</v>
       </c>
@@ -653,13 +716,48 @@
       <c r="F24">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <v>7822102021096</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="1">
+        <v>7822102021102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4500144690</v>
+      </c>
+      <c r="B26">
+        <v>19048183262</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="H26" s="3">
+        <v>7201902266188</v>
+      </c>
+      <c r="I26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H27" s="3">
+        <v>7201902266645</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H28" s="3">
+        <v>7611501611126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -679,7 +777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>

</xml_diff>